<commit_message>
Updated specification for IMX214 and OV7251 cameras Removed the 1.5V power supply from the assembly documents
</commit_message>
<xml_diff>
--- a/DM1095_OAK-D-LITE-DEV_DepthAI_USB3C/Docs/Assembly Outputs/BOM/BOM-DM1095(Production).xlsx
+++ b/DM1095_OAK-D-LITE-DEV_DepthAI_USB3C/Docs/Assembly Outputs/BOM/BOM-DM1095(Production).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="37395" windowHeight="19995"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="12435" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-DM1095(Production)" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="185">
   <si>
     <t>Name</t>
   </si>
@@ -57,7 +57,7 @@
     <t>0.1uF 0402</t>
   </si>
   <si>
-    <t>C1, C3, C5, C7, C9, C11, C23, C25, C27, C44, C45, C46, C49</t>
+    <t>C1, C3, C5, C7, C9, C11, C23, C25, C27, C44, C45, C46</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 10V X7R 0402 5%</t>
@@ -75,7 +75,7 @@
     <t>10uF 0603</t>
   </si>
   <si>
-    <t>C2, C4, C6, C8, C10, C12, C15, C17, C18, C19, C20, C21, C24, C26, C28, C38, C39, C42, C43</t>
+    <t>C2, C4, C6, C8, C10, C12, C15, C17, C18, C19, C20, C21, C24, C26, C28, C42, C43</t>
   </si>
   <si>
     <t>CAP CER 10UF 10V X5R 0603 20%</t>
@@ -204,7 +204,7 @@
     <t>600R/100MHz</t>
   </si>
   <si>
-    <t>FB1, FB2, FB3, FB4, FB5, FB6, FB7, FB8, FB9</t>
+    <t>FB1, FB2, FB3, FB4, FB5, FB7, FB8</t>
   </si>
   <si>
     <t>FERRITE BEAD, 0.1OHM, 2A, 0805, 600R/100MHz</t>
@@ -405,7 +405,7 @@
     <t>45.3K 0402</t>
   </si>
   <si>
-    <t>R8, R37</t>
+    <t>R8</t>
   </si>
   <si>
     <t>RES SMD 45.3K OHM 1% 1/16W 0402</t>
@@ -550,18 +550,6 @@
   </si>
   <si>
     <t>TUSB321RWBR</t>
-  </si>
-  <si>
-    <t>TLV70015DCK</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>Fixed Positive LDO Regulator, 1.5V, PMOS, PDSO5</t>
-  </si>
-  <si>
-    <t>TLV70015DCKR</t>
   </si>
   <si>
     <t>BNO085</t>
@@ -950,7 +938,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1006,7 +994,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -1037,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
@@ -1316,7 +1304,7 @@
         <v>60</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>61</v>
@@ -1731,7 +1719,7 @@
         <v>127</v>
       </c>
       <c r="B25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>128</v>
@@ -2097,10 +2085,10 @@
         <v>179</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>177</v>
@@ -2145,40 +2133,9 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>